<commit_message>
eer diagram completed, excel sheet updated, 'planning for analysis' nearly completed
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9A7A678-EFCE-4AAC-B0C8-16A175CC4781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A436AA4-6A27-4F8B-8BC2-AF4C17AAE69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="93">
   <si>
     <t>table_name</t>
   </si>
@@ -389,7 +389,29 @@
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -702,26 +724,28 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -793,6 +817,12 @@
       <c r="H2" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -819,6 +849,12 @@
       <c r="H3" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -897,6 +933,12 @@
       <c r="H6" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -923,6 +965,12 @@
       <c r="H7" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="J7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -947,7 +995,13 @@
         <v>92</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -973,7 +1027,13 @@
         <v>92</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1027,6 +1087,12 @@
       <c r="H11" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="J11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1053,6 +1119,12 @@
       <c r="H12" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="J12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1079,6 +1151,12 @@
       <c r="H13" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="J13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -1105,6 +1183,12 @@
       <c r="H14" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="J14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -1158,7 +1242,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1180,8 +1264,17 @@
       <c r="G17" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1197,8 +1290,23 @@
       <c r="E18" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1214,8 +1322,23 @@
       <c r="E19" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
@@ -1231,8 +1354,23 @@
       <c r="E20" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1248,8 +1386,23 @@
       <c r="E21" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1265,8 +1418,23 @@
       <c r="E22" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1282,8 +1450,23 @@
       <c r="E23" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1299,8 +1482,17 @@
       <c r="E24" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1316,8 +1508,23 @@
       <c r="E25" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1333,8 +1540,23 @@
       <c r="E26" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1350,8 +1572,23 @@
       <c r="E27" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1367,8 +1604,23 @@
       <c r="E28" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1384,8 +1636,17 @@
       <c r="E29" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1401,8 +1662,17 @@
       <c r="E30" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1418,8 +1688,17 @@
       <c r="E31" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1435,8 +1714,17 @@
       <c r="E32" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -1452,8 +1740,17 @@
       <c r="E33" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -1469,8 +1766,17 @@
       <c r="E34" s="1">
         <v>510</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
@@ -1486,8 +1792,23 @@
       <c r="E35" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J35" t="s">
+        <v>92</v>
+      </c>
+      <c r="K35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
@@ -1503,8 +1824,23 @@
       <c r="E36" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J36" t="s">
+        <v>92</v>
+      </c>
+      <c r="K36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
@@ -1520,8 +1856,23 @@
       <c r="E37" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1537,8 +1888,23 @@
       <c r="E38" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1554,8 +1920,23 @@
       <c r="E39" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1571,8 +1952,23 @@
       <c r="E40" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1588,8 +1984,23 @@
       <c r="E41" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -1605,8 +2016,23 @@
       <c r="E42" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
@@ -1622,8 +2048,23 @@
       <c r="E43" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -1639,8 +2080,23 @@
       <c r="E44" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>53</v>
       </c>
@@ -1656,8 +2112,23 @@
       <c r="E45" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -1673,8 +2144,23 @@
       <c r="E46" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
@@ -1690,8 +2176,23 @@
       <c r="E47" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -1707,8 +2208,23 @@
       <c r="E48" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -1724,8 +2240,23 @@
       <c r="E49" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
@@ -1741,8 +2272,23 @@
       <c r="E50" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
@@ -1758,8 +2304,17 @@
       <c r="E51" s="2">
         <v>120</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
@@ -1775,8 +2330,23 @@
       <c r="E52" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>53</v>
       </c>
@@ -1792,8 +2362,23 @@
       <c r="E53" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -1809,8 +2394,23 @@
       <c r="E54" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -1826,8 +2426,23 @@
       <c r="E55" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1843,8 +2458,23 @@
       <c r="E56" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -1860,8 +2490,23 @@
       <c r="E57" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1877,8 +2522,23 @@
       <c r="E58" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
@@ -1894,8 +2554,23 @@
       <c r="E59" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -1911,8 +2586,23 @@
       <c r="E60" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
@@ -1928,8 +2618,23 @@
       <c r="E61" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
@@ -1945,8 +2650,23 @@
       <c r="E62" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
@@ -1962,8 +2682,23 @@
       <c r="E63" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
@@ -1979,8 +2714,23 @@
       <c r="E64" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
@@ -1996,8 +2746,23 @@
       <c r="E65" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>22</v>
       </c>
@@ -2013,8 +2778,23 @@
       <c r="E66" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>22</v>
       </c>
@@ -2030,8 +2810,17 @@
       <c r="E67" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>76</v>
       </c>
@@ -2047,8 +2836,23 @@
       <c r="E68" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>76</v>
       </c>
@@ -2064,8 +2868,23 @@
       <c r="E69" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
@@ -2081,8 +2900,17 @@
       <c r="E70" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>78</v>
       </c>
@@ -2098,8 +2926,23 @@
       <c r="E71" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>78</v>
       </c>
@@ -2115,8 +2958,23 @@
       <c r="E72" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -2132,8 +2990,23 @@
       <c r="E73" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
@@ -2149,8 +3022,23 @@
       <c r="E74" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>78</v>
       </c>
@@ -2166,8 +3054,17 @@
       <c r="E75" s="2">
         <v>120</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -2183,8 +3080,23 @@
       <c r="E76" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
@@ -2200,8 +3112,23 @@
       <c r="E77" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
@@ -2217,8 +3144,23 @@
       <c r="E78" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -2234,8 +3176,23 @@
       <c r="E79" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
@@ -2251,8 +3208,17 @@
       <c r="E80" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>78</v>
       </c>
@@ -2268,8 +3234,17 @@
       <c r="E81" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>78</v>
       </c>
@@ -2285,8 +3260,17 @@
       <c r="E82" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -2302,8 +3286,23 @@
       <c r="E83" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>80</v>
       </c>
@@ -2319,8 +3318,17 @@
       <c r="E84" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>80</v>
       </c>
@@ -2336,8 +3344,41 @@
       <c r="E85" s="1">
         <v>4</v>
       </c>
+      <c r="F85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J14">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",J14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="containsText" priority="3" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:K85">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
exercise 2B completed, exercise 3A step 1 completed
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A436AA4-6A27-4F8B-8BC2-AF4C17AAE69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D285E347-9DF3-417E-95EF-DECA41EA6809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="147">
   <si>
     <t>table_name</t>
   </si>
@@ -314,6 +314,168 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Customer Contact</t>
+  </si>
+  <si>
+    <t>Customer Contact Title</t>
+  </si>
+  <si>
+    <t>Customer City</t>
+  </si>
+  <si>
+    <t>Customer Region</t>
+  </si>
+  <si>
+    <t>Customer Country</t>
+  </si>
+  <si>
+    <t>Employee Title</t>
+  </si>
+  <si>
+    <t>Employee City</t>
+  </si>
+  <si>
+    <t>Employee Region</t>
+  </si>
+  <si>
+    <t>Employee Country</t>
+  </si>
+  <si>
+    <t>Customer PostalCode</t>
+  </si>
+  <si>
+    <t>Employee LastName</t>
+  </si>
+  <si>
+    <t>Employee FirstName</t>
+  </si>
+  <si>
+    <t>Employee TitleOfCourtesy</t>
+  </si>
+  <si>
+    <t>Employee BirthDate</t>
+  </si>
+  <si>
+    <t>Employee HireDate</t>
+  </si>
+  <si>
+    <t>Employee PostalCode</t>
+  </si>
+  <si>
+    <t>Products UnitsInStock</t>
+  </si>
+  <si>
+    <t>Products UnitsOnOrder</t>
+  </si>
+  <si>
+    <t>Products ReorderLevel</t>
+  </si>
+  <si>
+    <t>Products Discontinued</t>
+  </si>
+  <si>
+    <t>Supplier City</t>
+  </si>
+  <si>
+    <t>Supplier Region</t>
+  </si>
+  <si>
+    <t>Supplier PostalCode</t>
+  </si>
+  <si>
+    <t>Supplier Country</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Sales Quantity</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Sales Discount Percent</t>
+  </si>
+  <si>
+    <t>Order Required Date</t>
+  </si>
+  <si>
+    <t>Order Shipped Date</t>
+  </si>
+  <si>
+    <t>Order Freight Amount</t>
+  </si>
+  <si>
+    <t>Order Ship Name</t>
+  </si>
+  <si>
+    <t>Order Ship City</t>
+  </si>
+  <si>
+    <t>Order Ship Region</t>
+  </si>
+  <si>
+    <t>Order Ship Postal Code</t>
+  </si>
+  <si>
+    <t>Order Ship Country</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Products Unit Price</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Supplier Contact</t>
+  </si>
+  <si>
+    <t>Supplier Contact Title</t>
+  </si>
+  <si>
+    <t>Territory</t>
+  </si>
+  <si>
+    <t>Employee ReportsTo EmployeeID</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Employee Age, Age at time of Sale</t>
+  </si>
+  <si>
+    <t>Years Employeed</t>
+  </si>
+  <si>
+    <t>Sales Amount, Discount Amount</t>
+  </si>
+  <si>
+    <t>Discount Amount</t>
+  </si>
+  <si>
+    <t>Product Availability</t>
   </si>
 </sst>
 </file>
@@ -377,11 +539,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -393,14 +556,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -727,7 +890,7 @@
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomRight" activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,13 +901,13 @@
     <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -849,6 +1012,9 @@
       <c r="H3" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="J3" s="1" t="s">
         <v>92</v>
       </c>
@@ -965,6 +1131,9 @@
       <c r="H7" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="J7" s="1" t="s">
         <v>92</v>
       </c>
@@ -997,6 +1166,9 @@
       <c r="H8" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I8" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="J8" s="1" t="s">
         <v>92</v>
       </c>
@@ -1029,6 +1201,9 @@
       <c r="H9" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I9" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="J9" s="1" t="s">
         <v>92</v>
       </c>
@@ -1087,6 +1262,9 @@
       <c r="H11" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I11" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="J11" s="1" t="s">
         <v>92</v>
       </c>
@@ -1119,6 +1297,9 @@
       <c r="H12" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I12" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="J12" s="1" t="s">
         <v>92</v>
       </c>
@@ -1151,11 +1332,14 @@
       <c r="H13" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I13" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="J13" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1183,6 +1367,9 @@
       <c r="H14" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I14" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="J14" s="1" t="s">
         <v>92</v>
       </c>
@@ -1215,6 +1402,7 @@
       <c r="H15" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -1241,8 +1429,9 @@
       <c r="H16" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1267,6 +1456,7 @@
       <c r="H17" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I17" s="4"/>
       <c r="J17" s="1" t="s">
         <v>92</v>
       </c>
@@ -1274,7 +1464,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1299,6 +1489,9 @@
       <c r="H18" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I18" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="J18" s="1" t="s">
         <v>92</v>
       </c>
@@ -1306,7 +1499,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1331,6 +1524,9 @@
       <c r="H19" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I19" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="J19" s="1" t="s">
         <v>92</v>
       </c>
@@ -1338,7 +1534,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
@@ -1363,6 +1559,9 @@
       <c r="H20" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I20" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="J20" s="1" t="s">
         <v>92</v>
       </c>
@@ -1370,7 +1569,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1395,6 +1594,9 @@
       <c r="H21" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I21" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="J21" s="1" t="s">
         <v>92</v>
       </c>
@@ -1402,7 +1604,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1427,14 +1629,23 @@
       <c r="H22" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I22" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="J22" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1459,14 +1670,23 @@
       <c r="H23" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I23" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="J23" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1491,8 +1711,9 @@
       <c r="H24" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1517,6 +1738,9 @@
       <c r="H25" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I25" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="J25" s="1" t="s">
         <v>92</v>
       </c>
@@ -1524,7 +1748,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1549,6 +1773,9 @@
       <c r="H26" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I26" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="J26" s="1" t="s">
         <v>92</v>
       </c>
@@ -1556,7 +1783,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1581,14 +1808,17 @@
       <c r="H27" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I27" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="J27" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1613,6 +1843,9 @@
       <c r="H28" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I28" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="J28" s="1" t="s">
         <v>92</v>
       </c>
@@ -1620,7 +1853,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1645,8 +1878,9 @@
       <c r="H29" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1671,8 +1905,9 @@
       <c r="H30" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1697,8 +1932,9 @@
       <c r="H31" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1723,8 +1959,9 @@
       <c r="H32" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -1744,13 +1981,16 @@
         <v>92</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -1775,8 +2015,9 @@
       <c r="H34" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
@@ -1801,6 +2042,7 @@
       <c r="H35" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I35" s="4"/>
       <c r="J35" t="s">
         <v>92</v>
       </c>
@@ -1808,7 +2050,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
@@ -1833,6 +2075,7 @@
       <c r="H36" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I36" s="4"/>
       <c r="J36" t="s">
         <v>92</v>
       </c>
@@ -1840,7 +2083,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
@@ -1865,6 +2108,7 @@
       <c r="H37" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I37" s="4"/>
       <c r="J37" s="1" t="s">
         <v>92</v>
       </c>
@@ -1872,7 +2116,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1897,6 +2141,7 @@
       <c r="H38" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I38" s="4"/>
       <c r="J38" s="1" t="s">
         <v>92</v>
       </c>
@@ -1904,7 +2149,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1929,14 +2174,23 @@
       <c r="H39" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I39" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="J39" s="1" t="s">
         <v>91</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1961,14 +2215,23 @@
       <c r="H40" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I40" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="J40" s="1" t="s">
         <v>91</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1993,14 +2256,23 @@
       <c r="H41" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I41" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="J41" s="1" t="s">
         <v>91</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -2032,7 +2304,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
@@ -2064,7 +2336,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -2096,7 +2368,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>53</v>
       </c>
@@ -2121,14 +2393,20 @@
       <c r="H45" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I45" t="s">
+        <v>121</v>
+      </c>
       <c r="J45" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -2153,14 +2431,20 @@
       <c r="H46" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I46" t="s">
+        <v>123</v>
+      </c>
       <c r="J46" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
@@ -2185,14 +2469,20 @@
       <c r="H47" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I47" t="s">
+        <v>124</v>
+      </c>
       <c r="J47" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -2212,11 +2502,14 @@
         <v>92</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I48" t="s">
+        <v>77</v>
+      </c>
       <c r="J48" s="1" t="s">
         <v>92</v>
       </c>
@@ -2224,7 +2517,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -2249,14 +2542,20 @@
       <c r="H49" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I49" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="J49" s="1" t="s">
         <v>91</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L49" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
@@ -2281,6 +2580,9 @@
       <c r="H50" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I50" t="s">
+        <v>126</v>
+      </c>
       <c r="J50" s="1" t="s">
         <v>92</v>
       </c>
@@ -2288,7 +2590,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
@@ -2314,7 +2616,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
@@ -2339,6 +2641,9 @@
       <c r="H52" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I52" t="s">
+        <v>127</v>
+      </c>
       <c r="J52" s="1" t="s">
         <v>92</v>
       </c>
@@ -2346,7 +2651,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>53</v>
       </c>
@@ -2371,6 +2676,9 @@
       <c r="H53" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I53" t="s">
+        <v>128</v>
+      </c>
       <c r="J53" s="1" t="s">
         <v>92</v>
       </c>
@@ -2378,7 +2686,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -2403,14 +2711,17 @@
       <c r="H54" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I54" t="s">
+        <v>129</v>
+      </c>
       <c r="J54" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -2435,6 +2746,9 @@
       <c r="H55" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I55" t="s">
+        <v>130</v>
+      </c>
       <c r="J55" s="1" t="s">
         <v>92</v>
       </c>
@@ -2442,7 +2756,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -2467,6 +2781,7 @@
       <c r="H56" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I56" s="4"/>
       <c r="J56" s="1" t="s">
         <v>92</v>
       </c>
@@ -2474,7 +2789,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -2499,6 +2814,9 @@
       <c r="H57" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I57" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="J57" s="1" t="s">
         <v>92</v>
       </c>
@@ -2506,7 +2824,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -2531,6 +2849,7 @@
       <c r="H58" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I58" s="4"/>
       <c r="J58" s="1" t="s">
         <v>92</v>
       </c>
@@ -2538,7 +2857,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
@@ -2563,6 +2882,7 @@
       <c r="H59" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I59" s="4"/>
       <c r="J59" s="1" t="s">
         <v>92</v>
       </c>
@@ -2570,7 +2890,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -2595,6 +2915,7 @@
       <c r="H60" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I60" s="4"/>
       <c r="J60" s="1" t="s">
         <v>91</v>
       </c>
@@ -2602,7 +2923,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
@@ -2627,14 +2948,20 @@
       <c r="H61" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I61" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="J61" s="1" t="s">
         <v>91</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
@@ -2659,14 +2986,23 @@
       <c r="H62" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I62" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="J62" s="1" t="s">
         <v>91</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
@@ -2691,14 +3027,20 @@
       <c r="H63" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I63" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="J63" s="1" t="s">
         <v>91</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
@@ -2723,14 +3065,20 @@
       <c r="H64" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I64" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="J64" s="1" t="s">
         <v>91</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
@@ -2755,14 +3103,20 @@
       <c r="H65" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I65" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="J65" s="1" t="s">
         <v>91</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>22</v>
       </c>
@@ -2794,7 +3148,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>22</v>
       </c>
@@ -2819,8 +3173,11 @@
       <c r="H67" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I67" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>76</v>
       </c>
@@ -2845,14 +3202,15 @@
       <c r="H68" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I68" s="4"/>
       <c r="J68" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>76</v>
       </c>
@@ -2877,6 +3235,7 @@
       <c r="H69" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I69" s="4"/>
       <c r="J69" s="1" t="s">
         <v>92</v>
       </c>
@@ -2884,7 +3243,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
@@ -2909,8 +3268,9 @@
       <c r="H70" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>78</v>
       </c>
@@ -2935,6 +3295,7 @@
       <c r="H71" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I71" s="4"/>
       <c r="J71" s="1" t="s">
         <v>92</v>
       </c>
@@ -2942,7 +3303,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>78</v>
       </c>
@@ -2967,6 +3328,9 @@
       <c r="H72" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I72" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="J72" s="1" t="s">
         <v>92</v>
       </c>
@@ -2974,7 +3338,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -2999,6 +3363,9 @@
       <c r="H73" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I73" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="J73" s="1" t="s">
         <v>92</v>
       </c>
@@ -3006,7 +3373,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
@@ -3031,6 +3398,9 @@
       <c r="H74" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I74" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="J74" s="1" t="s">
         <v>92</v>
       </c>
@@ -3038,7 +3408,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>78</v>
       </c>
@@ -3063,8 +3433,9 @@
       <c r="H75" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I75" s="4"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -3089,6 +3460,9 @@
       <c r="H76" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I76" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="J76" s="1" t="s">
         <v>92</v>
       </c>
@@ -3096,7 +3470,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
@@ -3121,6 +3495,9 @@
       <c r="H77" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I77" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="J77" s="1" t="s">
         <v>92</v>
       </c>
@@ -3128,7 +3505,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
@@ -3153,14 +3530,17 @@
       <c r="H78" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I78" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="J78" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -3185,6 +3565,9 @@
       <c r="H79" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I79" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="J79" s="1" t="s">
         <v>92</v>
       </c>
@@ -3192,7 +3575,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
@@ -3217,6 +3600,7 @@
       <c r="H80" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="I80" s="4"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
@@ -3243,6 +3627,7 @@
       <c r="H81" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="I81" s="4"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
@@ -3269,6 +3654,7 @@
       <c r="H82" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="I82" s="4"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
@@ -3295,6 +3681,7 @@
       <c r="H83" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I83" s="4"/>
       <c r="J83" s="1" t="s">
         <v>92</v>
       </c>
@@ -3327,6 +3714,12 @@
       <c r="H84" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="I84" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
@@ -3353,6 +3746,7 @@
       <c r="H85" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="I85" s="4"/>
       <c r="J85" s="1" t="s">
         <v>92</v>
       </c>
@@ -3361,22 +3755,22 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J14">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="yes">
-      <formula>NOT(ISERROR(SEARCH("yes",J14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" priority="3" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="yes">
+    <cfRule type="containsText" priority="3" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:K85">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",J14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3384,34 +3778,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA5D0A6329BB324E86983B32928CFC2E" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b28f3bc5995c0091f528145aa367664">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xmlns:ns3="ced60a7f-99b1-48d2-b555-34851c8026ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48800952b0413791e1a5c8543532e00d" ns2:_="" ns3:_="">
     <xsd:import namespace="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
@@ -3652,26 +4018,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0257D61C-6042-483B-9C34-3DE0D82CB154}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
-    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0F2F57-CFBB-4DE2-9688-0C0C6A435162}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3688,4 +4063,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0257D61C-6042-483B-9C34-3DE0D82CB154}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
+    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
exercise 3A step 3 and step 4 completed
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D285E347-9DF3-417E-95EF-DECA41EA6809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2BB5C1-0E56-4C11-8F72-F7B38AE93C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
@@ -887,10 +887,10 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M64" sqref="M64"/>
+      <selection pane="bottomRight" activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3171,7 +3171,7 @@
         <v>92</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I67" t="s">
         <v>22</v>
@@ -3712,7 +3712,7 @@
         <v>92</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I84" s="4" t="s">
         <v>136</v>
@@ -4019,15 +4019,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
@@ -4044,6 +4035,15 @@
     <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4066,14 +4066,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0257D61C-6042-483B-9C34-3DE0D82CB154}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4082,4 +4074,12 @@
     <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0257D61C-6042-483B-9C34-3DE0D82CB154}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>